<commit_message>
Addition of filtering option + fixing orientation
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s.prasannachandran/Documents/Upwork_Maps_Visualization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E392F85-0A7D-7C42-857B-69B29E6477D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E0373E-B467-D94D-AB94-C0F9CFD743CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16640" xr2:uid="{6BB020FE-AFA3-5E49-987D-E57C3925B7BE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>lat</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>VVVV</t>
+  </si>
+  <si>
+    <t>revenue</t>
   </si>
 </sst>
 </file>
@@ -463,15 +466,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ABE427-C4F4-C545-BDB1-DF03D1A156C1}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -484,8 +487,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -498,8 +504,11 @@
       <c r="D2">
         <v>11.793518000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -512,8 +521,11 @@
       <c r="D3">
         <v>11.824657999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -526,8 +538,11 @@
       <c r="D4">
         <v>11.704912999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -540,8 +555,11 @@
       <c r="D5">
         <v>11.596809</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -554,8 +572,11 @@
       <c r="D6">
         <v>11.486039999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -568,8 +589,11 @@
       <c r="D7">
         <v>11.384065</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -582,8 +606,11 @@
       <c r="D8">
         <v>11.316371</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -596,8 +623,11 @@
       <c r="D9">
         <v>11.282776999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -610,8 +640,11 @@
       <c r="D10">
         <v>11.25836</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -624,8 +657,11 @@
       <c r="D11">
         <v>11.32372</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -638,8 +674,11 @@
       <c r="D12">
         <v>11.33221</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -652,8 +691,11 @@
       <c r="D13">
         <v>11.436249999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -666,8 +708,11 @@
       <c r="D14">
         <v>11.650613999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -680,8 +725,11 @@
       <c r="D15">
         <v>11.862667999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -694,8 +742,11 @@
       <c r="D16">
         <v>11.995403</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -708,8 +759,11 @@
       <c r="D17">
         <v>12.212127000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -722,8 +776,11 @@
       <c r="D18">
         <v>12.299982999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -736,8 +793,11 @@
       <c r="D19">
         <v>12.390628</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -750,8 +810,11 @@
       <c r="D20">
         <v>12.4342785</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -764,8 +827,11 @@
       <c r="D21">
         <v>12.493862999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -778,8 +844,11 @@
       <c r="D22">
         <v>12.554451</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -791,6 +860,9 @@
       </c>
       <c r="D23">
         <v>12.594722000000001</v>
+      </c>
+      <c r="E23">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>